<commit_message>
Fix column width when displayed on DataGridView
</commit_message>
<xml_diff>
--- a/QuanLyDienNang/Templates/NhapThongTinKhachHang_Sample.xlsx
+++ b/QuanLyDienNang/Templates/NhapThongTinKhachHang_Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\QuanLyDienNang\QuanLyDienNang\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA737737-2D52-44ED-AD3C-05885A7C0FA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938BB97-383D-456D-9A6C-C8F272B9FBC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="23985" windowHeight="12825" xr2:uid="{13172063-5E7C-438F-A150-65B67473061E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{13172063-5E7C-438F-A150-65B67473061E}"/>
   </bookViews>
   <sheets>
     <sheet name="DNTT" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>HoVaTen</t>
   </si>
@@ -154,6 +154,48 @@
   </si>
   <si>
     <t>0567891234</t>
+  </si>
+  <si>
+    <t>HD2468013579</t>
+  </si>
+  <si>
+    <t>HD2468013580</t>
+  </si>
+  <si>
+    <t>HD2468013581</t>
+  </si>
+  <si>
+    <t>HD2468013582</t>
+  </si>
+  <si>
+    <t>HD2468013583</t>
+  </si>
+  <si>
+    <t>HD2468013584</t>
+  </si>
+  <si>
+    <t>ABCXYZ</t>
+  </si>
+  <si>
+    <t>5907000000001</t>
+  </si>
+  <si>
+    <t>5907000000002</t>
+  </si>
+  <si>
+    <t>5907000000003</t>
+  </si>
+  <si>
+    <t>5907000000004</t>
+  </si>
+  <si>
+    <t>5907000000005</t>
+  </si>
+  <si>
+    <t>5907000000006</t>
+  </si>
+  <si>
+    <t>Vietcombank</t>
   </si>
 </sst>
 </file>
@@ -212,12 +254,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -536,7 +579,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H7"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,13 +589,14 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -619,14 +663,29 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>1234567890</v>
+      </c>
       <c r="H2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
       <c r="K2" s="3">
         <v>44185</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -648,14 +707,29 @@
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3">
+        <v>1234567891</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
       <c r="K3" s="3">
         <v>44186</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -677,14 +751,29 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4">
+        <v>1234567892</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
       <c r="K4" s="3">
         <v>44187</v>
+      </c>
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -706,14 +795,29 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5">
+        <v>1234567893</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
       <c r="K5" s="3">
         <v>44188</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -735,14 +839,29 @@
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6">
+        <v>1234567894</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
       <c r="K6" s="3">
         <v>44189</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -764,14 +883,29 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="G7">
+        <v>1234567895</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
       <c r="K7" s="3">
         <v>44190</v>
+      </c>
+      <c r="L7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>